<commit_message>
added indexing for files
</commit_message>
<xml_diff>
--- a/test/data/test-file.xlsx
+++ b/test/data/test-file.xlsx
@@ -1,433 +1,417 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="TestSheet" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="TestObject" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="TestList" sheetId="3" state="visible" r:id="rId5"/>
-    <sheet name="InconsistentSheetName_" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet sheetId="1" name="TestSheet" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="TestObject" state="visible" r:id="rId5"/>
+    <sheet sheetId="3" name="TestList" state="visible" r:id="rId6"/>
+    <sheet sheetId="4" name="InconsistentSheetName_" state="visible" r:id="rId7"/>
+    <sheet sheetId="5" name="Indexing" state="visible" r:id="rId8"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="R1C1" iterate="false" iterateDelta="0.0001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="111">
   <si>
-    <t xml:space="preserve">scoring</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aaaaaaaaaa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">exact</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aaaaaaaaab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inconsistent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aaaaaaaabc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aaaaaaabcd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aaaaaabcde</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aaaaabcdef</t>
-  </si>
-  <si>
-    <t xml:space="preserve">missing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aaaabcdefg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aaabcdefgh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aabcdefghi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">abcdefghij</t>
-  </si>
-  <si>
-    <t xml:space="preserve">position</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pos1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">logical</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$and</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$or</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aa,bb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ee,ff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NoErrors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">two</t>
-  </si>
-  <si>
-    <t xml:space="preserve">one</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">three</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">four</t>
-  </si>
-  <si>
-    <t xml:space="preserve">InconsistentHeaderName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sixss</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fivee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">seVenn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eight_</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MissingDataHeader</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data12</t>
+    <t>scoring</t>
+  </si>
+  <si>
+    <t>aaaaaaaaaa</t>
+  </si>
+  <si>
+    <t>exact</t>
+  </si>
+  <si>
+    <t>aaaaaaaaab</t>
+  </si>
+  <si>
+    <t>inconsistent</t>
+  </si>
+  <si>
+    <t>aaaaaaaabc</t>
+  </si>
+  <si>
+    <t>aaaaaaabcd</t>
+  </si>
+  <si>
+    <t>aaaaaabcde</t>
+  </si>
+  <si>
+    <t>aaaaabcdef</t>
+  </si>
+  <si>
+    <t>missing</t>
+  </si>
+  <si>
+    <t>aaaabcdefg</t>
+  </si>
+  <si>
+    <t>aaabcdefgh</t>
+  </si>
+  <si>
+    <t>aabcdefghi</t>
+  </si>
+  <si>
+    <t>abcdefghij</t>
+  </si>
+  <si>
+    <t>position</t>
+  </si>
+  <si>
+    <t>pos1</t>
+  </si>
+  <si>
+    <t>logical</t>
+  </si>
+  <si>
+    <t>aa</t>
+  </si>
+  <si>
+    <t>bb</t>
+  </si>
+  <si>
+    <t>$and</t>
+  </si>
+  <si>
+    <t>$or</t>
+  </si>
+  <si>
+    <t>aa,bb</t>
+  </si>
+  <si>
+    <t>cc</t>
+  </si>
+  <si>
+    <t>dd</t>
+  </si>
+  <si>
+    <t>ee,ff</t>
+  </si>
+  <si>
+    <t>gg</t>
+  </si>
+  <si>
+    <t>ee</t>
+  </si>
+  <si>
+    <t>hh</t>
+  </si>
+  <si>
+    <t>ff</t>
+  </si>
+  <si>
+    <t>NoErrors</t>
+  </si>
+  <si>
+    <t>two</t>
+  </si>
+  <si>
+    <t>one</t>
+  </si>
+  <si>
+    <t>data1</t>
+  </si>
+  <si>
+    <t>data2</t>
+  </si>
+  <si>
+    <t>data3</t>
+  </si>
+  <si>
+    <t>three</t>
+  </si>
+  <si>
+    <t>data4</t>
+  </si>
+  <si>
+    <t>four</t>
+  </si>
+  <si>
+    <t>InconsistentHeaderName</t>
+  </si>
+  <si>
+    <t>sixss</t>
+  </si>
+  <si>
+    <t>Fivee</t>
+  </si>
+  <si>
+    <t>data5</t>
+  </si>
+  <si>
+    <t>data6</t>
+  </si>
+  <si>
+    <t>data7</t>
+  </si>
+  <si>
+    <t>seVenn</t>
+  </si>
+  <si>
+    <t>data8</t>
+  </si>
+  <si>
+    <t>Eight_</t>
+  </si>
+  <si>
+    <t>MissingDataHeader</t>
+  </si>
+  <si>
+    <t>data9</t>
+  </si>
+  <si>
+    <t>data10</t>
+  </si>
+  <si>
+    <t>data11</t>
+  </si>
+  <si>
+    <t>data12</t>
   </si>
   <si>
     <t xml:space="preserve">IncorrectRowOffset </t>
   </si>
   <si>
-    <t xml:space="preserve">fourteen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">thirteen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fifteen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sixteen</t>
+    <t>fourteen</t>
+  </si>
+  <si>
+    <t>thirteen</t>
+  </si>
+  <si>
+    <t>data13</t>
+  </si>
+  <si>
+    <t>data14</t>
+  </si>
+  <si>
+    <t>data15</t>
+  </si>
+  <si>
+    <t>fifteen</t>
+  </si>
+  <si>
+    <t>data16</t>
+  </si>
+  <si>
+    <t>sixteen</t>
   </si>
   <si>
     <t xml:space="preserve">IncorrectColumnIndex </t>
   </si>
   <si>
-    <t xml:space="preserve">eighteen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">seventeen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nineteen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">twenty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MultiCellHeaders</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">five</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dataA1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dataB1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dataC1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dataA2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dataB2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dataC2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dataA3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dataB3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dataC3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fouRr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fiVe_</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Six!</t>
+    <t>eighteen</t>
+  </si>
+  <si>
+    <t>seventeen</t>
+  </si>
+  <si>
+    <t>data17</t>
+  </si>
+  <si>
+    <t>data18</t>
+  </si>
+  <si>
+    <t>data19</t>
+  </si>
+  <si>
+    <t>nineteen</t>
+  </si>
+  <si>
+    <t>data20</t>
+  </si>
+  <si>
+    <t>twenty</t>
+  </si>
+  <si>
+    <t>MultiCellHeaders</t>
+  </si>
+  <si>
+    <t>data22</t>
+  </si>
+  <si>
+    <t>data24</t>
+  </si>
+  <si>
+    <t>five</t>
+  </si>
+  <si>
+    <t>data25</t>
+  </si>
+  <si>
+    <t>data21</t>
+  </si>
+  <si>
+    <t>data23</t>
+  </si>
+  <si>
+    <t>dataA1</t>
+  </si>
+  <si>
+    <t>dataB1</t>
+  </si>
+  <si>
+    <t>dataC1</t>
+  </si>
+  <si>
+    <t>dataA2</t>
+  </si>
+  <si>
+    <t>dataB2</t>
+  </si>
+  <si>
+    <t>dataC2</t>
+  </si>
+  <si>
+    <t>dataA3</t>
+  </si>
+  <si>
+    <t>dataB3</t>
+  </si>
+  <si>
+    <t>dataC3</t>
+  </si>
+  <si>
+    <t>fouRr</t>
+  </si>
+  <si>
+    <t>fiVe_</t>
+  </si>
+  <si>
+    <t>Six!</t>
   </si>
   <si>
     <t xml:space="preserve">IncorrectRowIndex </t>
   </si>
   <si>
-    <t xml:space="preserve">ten</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eleven</t>
-  </si>
-  <si>
-    <t xml:space="preserve">twelve</t>
-  </si>
-  <si>
-    <t xml:space="preserve">seven</t>
-  </si>
-  <si>
-    <t xml:space="preserve">teen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dataC4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ddatC5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dataC6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nine9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Twentyy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">twe_ty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">one1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">twenty five</t>
-  </si>
-  <si>
-    <t xml:space="preserve">six</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Twenty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">twenty eight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">thir</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A sheet name is considered inconsistant if the sheets name scores less than 0.001 in a fuzzy search among all sheet names present.</t>
+    <t>ten</t>
+  </si>
+  <si>
+    <t>eleven</t>
+  </si>
+  <si>
+    <t>twelve</t>
+  </si>
+  <si>
+    <t>seven</t>
+  </si>
+  <si>
+    <t>teen</t>
+  </si>
+  <si>
+    <t>eight</t>
+  </si>
+  <si>
+    <t>dataC4</t>
+  </si>
+  <si>
+    <t>ddatC5</t>
+  </si>
+  <si>
+    <t>dataC6</t>
+  </si>
+  <si>
+    <t>nine9</t>
+  </si>
+  <si>
+    <t>Twentyy</t>
+  </si>
+  <si>
+    <t>twe_ty</t>
+  </si>
+  <si>
+    <t>one1</t>
+  </si>
+  <si>
+    <t>twenty five</t>
+  </si>
+  <si>
+    <t>six</t>
+  </si>
+  <si>
+    <t>Twenty</t>
+  </si>
+  <si>
+    <t>twenty eight</t>
+  </si>
+  <si>
+    <t>nine</t>
+  </si>
+  <si>
+    <t>thir</t>
+  </si>
+  <si>
+    <t>ty</t>
+  </si>
+  <si>
+    <t>Change</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
+      <color theme="1"/>
+      <family val="2"/>
+      <scheme val="minor"/>
       <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
+      <charset val="1"/>
+      <color theme="1"/>
+      <family val="2"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <charset val="1"/>
+      <family val="2"/>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
+      <charset val="1"/>
+      <color rgb="FF006600"/>
+      <family val="2"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <charset val="1"/>
+      <color rgb="FF996600"/>
+      <family val="2"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <charset val="1"/>
+      <color rgb="FFCC0000"/>
+      <family val="2"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <charset val="1"/>
+      <color rgb="FF006600"/>
+      <family val="2"/>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
+      <charset val="1"/>
+      <color rgb="FFCC0000"/>
+      <family val="2"/>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF996600"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006600"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFCC0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -439,14 +423,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -457,35 +441,35 @@
     </fill>
   </fills>
   <borders count="5">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin"/>
       <right/>
       <top style="thin"/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin"/>
       <right style="thin"/>
       <top/>
@@ -493,177 +477,70 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="bottom" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="bottom" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="bottom" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="bottom" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="bottom" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="22" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="22" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="bottom" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="bottom" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="bottom" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="bottom" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="bottom" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="bottom" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Neutral 1" xfId="20"/>
-    <cellStyle name="Gut" xfId="21"/>
-    <cellStyle name="Schlecht" xfId="22"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -774,127 +651,124 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B42" activeCellId="0" sqref="B42"/>
+    <sheetView workbookViewId="0" zoomScale="80" zoomScaleNormal="80" view="normal">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0" defaultColWidth="11.53515625" customHeight="1"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" ht="12.75" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" ht="12.75" customHeight="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="n">
-        <v>2.22044604925031E-016</v>
+      <c r="C4" s="3">
+        <v>2.22044604925031e-16</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" ht="12.75" customHeight="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="4" t="n">
+      <c r="C5" s="4">
         <v>0.1</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" ht="12.75" customHeight="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="4" t="n">
+      <c r="C6" s="4">
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" ht="12.75" customHeight="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="4" t="n">
+      <c r="C7" s="4">
         <v>0.3</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" ht="12.75" customHeight="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="4" t="n">
+      <c r="C8" s="4">
         <v>0.4</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" ht="12.75" customHeight="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="5" t="n">
+      <c r="C9" s="5">
         <v>0.5</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" ht="12.75" customHeight="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="5" t="n">
+      <c r="C10" s="5">
         <v>0.6</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" ht="12.75" customHeight="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="5" t="n">
+      <c r="C11" s="5">
         <v>0.7</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" ht="12.75" customHeight="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="5" t="n">
+      <c r="C12" s="5">
         <v>0.8</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" ht="12.75" customHeight="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="5" t="n">
+      <c r="C13" s="5">
         <v>0.9</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" ht="12.75" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="12.75" customHeight="1" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
-      <c r="F17" s="7" t="n">
+      <c r="F17" s="7">
         <v>4</v>
       </c>
       <c r="G17" s="6"/>
@@ -902,167 +776,167 @@
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
     </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" ht="12.75" customHeight="1" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
-      <c r="E18" s="7" t="n">
+      <c r="E18" s="7">
         <v>4</v>
       </c>
-      <c r="F18" s="7" t="n">
+      <c r="F18" s="7">
         <v>3</v>
       </c>
-      <c r="G18" s="7" t="n">
+      <c r="G18" s="7">
         <v>4</v>
       </c>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
     </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" ht="12.75" customHeight="1" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
-      <c r="D19" s="7" t="n">
+      <c r="D19" s="7">
         <v>4</v>
       </c>
-      <c r="E19" s="7" t="n">
+      <c r="E19" s="7">
         <v>3</v>
       </c>
-      <c r="F19" s="7" t="n">
+      <c r="F19" s="7">
         <v>2</v>
       </c>
-      <c r="G19" s="7" t="n">
+      <c r="G19" s="7">
         <v>3</v>
       </c>
-      <c r="H19" s="7" t="n">
+      <c r="H19" s="7">
         <v>4</v>
       </c>
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
     </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" ht="12.75" customHeight="1" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="6"/>
-      <c r="C20" s="7" t="n">
+      <c r="C20" s="7">
         <v>4</v>
       </c>
-      <c r="D20" s="7" t="n">
+      <c r="D20" s="7">
         <v>3</v>
       </c>
-      <c r="E20" s="7" t="n">
+      <c r="E20" s="7">
         <v>2</v>
       </c>
-      <c r="F20" s="7" t="n">
+      <c r="F20" s="7">
         <v>1</v>
       </c>
-      <c r="G20" s="7" t="n">
+      <c r="G20" s="7">
         <v>2</v>
       </c>
-      <c r="H20" s="7" t="n">
+      <c r="H20" s="7">
         <v>3</v>
       </c>
-      <c r="I20" s="7" t="n">
+      <c r="I20" s="7">
         <v>4</v>
       </c>
       <c r="J20" s="6"/>
     </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B21" s="7" t="n">
+    <row r="21" ht="12.75" customHeight="1" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="7">
         <v>4</v>
       </c>
-      <c r="C21" s="7" t="n">
+      <c r="C21" s="7">
         <v>3</v>
       </c>
-      <c r="D21" s="7" t="n">
+      <c r="D21" s="7">
         <v>2</v>
       </c>
-      <c r="E21" s="7" t="n">
+      <c r="E21" s="7">
         <v>1</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G21" s="7" t="n">
+      <c r="G21" s="7">
         <v>1</v>
       </c>
-      <c r="H21" s="7" t="n">
+      <c r="H21" s="7">
         <v>2</v>
       </c>
-      <c r="I21" s="7" t="n">
+      <c r="I21" s="7">
         <v>3</v>
       </c>
-      <c r="J21" s="7" t="n">
+      <c r="J21" s="7">
         <v>4</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" ht="12.75" customHeight="1" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
-      <c r="C22" s="7" t="n">
+      <c r="C22" s="7">
         <v>4</v>
       </c>
-      <c r="D22" s="7" t="n">
+      <c r="D22" s="7">
         <v>3</v>
       </c>
-      <c r="E22" s="7" t="n">
+      <c r="E22" s="7">
         <v>2</v>
       </c>
-      <c r="F22" s="7" t="n">
+      <c r="F22" s="7">
         <v>1</v>
       </c>
-      <c r="G22" s="7" t="n">
+      <c r="G22" s="7">
         <v>2</v>
       </c>
-      <c r="H22" s="7" t="n">
+      <c r="H22" s="7">
         <v>3</v>
       </c>
-      <c r="I22" s="7" t="n">
+      <c r="I22" s="7">
         <v>4</v>
       </c>
       <c r="J22" s="6"/>
     </row>
-    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" ht="12.75" customHeight="1" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
-      <c r="D23" s="7" t="n">
+      <c r="D23" s="7">
         <v>4</v>
       </c>
-      <c r="E23" s="7" t="n">
+      <c r="E23" s="7">
         <v>3</v>
       </c>
-      <c r="F23" s="7" t="n">
+      <c r="F23" s="7">
         <v>2</v>
       </c>
-      <c r="G23" s="7" t="n">
+      <c r="G23" s="7">
         <v>3</v>
       </c>
-      <c r="H23" s="7" t="n">
+      <c r="H23" s="7">
         <v>4</v>
       </c>
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
     </row>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" ht="12.75" customHeight="1" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
-      <c r="E24" s="7" t="n">
+      <c r="E24" s="7">
         <v>4</v>
       </c>
-      <c r="F24" s="7" t="n">
+      <c r="F24" s="7">
         <v>3</v>
       </c>
-      <c r="G24" s="7" t="n">
+      <c r="G24" s="7">
         <v>4</v>
       </c>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
     </row>
-    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" ht="12.75" customHeight="1" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
-      <c r="F25" s="7" t="n">
+      <c r="F25" s="7">
         <v>4</v>
       </c>
       <c r="G25" s="6"/>
@@ -1070,14 +944,14 @@
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" ht="12.75" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="28" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" ht="12.75" customHeight="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="9" t="s">
         <v>17</v>
       </c>
@@ -1091,12 +965,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="30" ht="12.75" customHeight="1" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E30" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" ht="12.75" customHeight="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="9" t="s">
         <v>22</v>
       </c>
@@ -1105,12 +979,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="32" ht="12.75" customHeight="1" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E32" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" ht="12.75" customHeight="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="9"/>
       <c r="C33" s="10" t="s">
         <v>23</v>
@@ -1119,12 +993,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="34" ht="12.75" customHeight="1" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E34" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="35" ht="12.75" customHeight="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="11" t="s">
         <v>26</v>
       </c>
@@ -1132,34 +1006,33 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="36" ht="12.75" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="37" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="12.75" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" s="11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="39" ht="12.75" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" s="12"/>
     </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="40" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="12.75" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" s="11"/>
     </row>
-    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="42" ht="12.75" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" s="12" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
   </headerFooter>
@@ -1167,31 +1040,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B33" activeCellId="0" sqref="B33"/>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100" view="normal">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0" defaultColWidth="11.53515625" customHeight="1"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" ht="12.75" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" ht="12.75" customHeight="1" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D4" s="13" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" ht="12.75" customHeight="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="13" t="s">
         <v>31</v>
       </c>
@@ -1211,24 +1081,24 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" ht="12.75" customHeight="1" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G6" s="13" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" ht="12.75" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" ht="12.75" customHeight="1" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D10" s="14" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" ht="12.75" customHeight="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="14" t="s">
         <v>40</v>
       </c>
@@ -1248,22 +1118,22 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" ht="12.75" customHeight="1" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G12" s="14" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" ht="12.75" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" ht="12.75" customHeight="1" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D16" s="14"/>
     </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" ht="12.75" customHeight="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="14"/>
       <c r="C17" s="2" t="s">
         <v>48</v>
@@ -1279,27 +1149,27 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" ht="12.75" customHeight="1" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G18" s="14"/>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="12.75" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="12.75" customHeight="1" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D22" s="13"/>
     </row>
-    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" ht="12.75" customHeight="1" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="13"/>
       <c r="D23" s="14" t="s">
         <v>53</v>
       </c>
       <c r="F23" s="13"/>
     </row>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" ht="12.75" customHeight="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="14" t="s">
         <v>54</v>
       </c>
@@ -1319,24 +1189,24 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" ht="12.75" customHeight="1" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G25" s="14" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" ht="12.75" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="28" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" ht="12.75" customHeight="1" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E29" s="14" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="30" ht="12.75" customHeight="1" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C30" s="14" t="s">
         <v>63</v>
       </c>
@@ -1356,19 +1226,19 @@
         <v>68</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" ht="12.75" customHeight="1" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H31" s="14" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="12.75" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="34" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="12.75" customHeight="1" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B35" s="13" t="s">
         <v>69</v>
       </c>
@@ -1396,7 +1266,7 @@
       <c r="L35" s="13"/>
       <c r="M35" s="13"/>
     </row>
-    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="36" ht="12.75" customHeight="1" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B36" s="13" t="s">
         <v>31</v>
       </c>
@@ -1411,7 +1281,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="37" ht="12.75" customHeight="1" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
         <v>75</v>
       </c>
@@ -1419,21 +1289,20 @@
         <v>69</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="38" ht="12.75" customHeight="1" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F38" s="14" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="39" ht="12.75" customHeight="1" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F39" s="2" t="s">
         <v>76</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
   </headerFooter>
@@ -1441,28 +1310,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I78"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F65" activeCellId="0" sqref="F65"/>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100" view="normal">
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0" defaultColWidth="11.53515625" customHeight="1"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" ht="12.75" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" ht="12.75" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" ht="12.75" customHeight="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
         <v>31</v>
       </c>
@@ -1473,7 +1339,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" ht="12.75" customHeight="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>77</v>
       </c>
@@ -1484,7 +1350,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" ht="12.75" customHeight="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>80</v>
       </c>
@@ -1495,7 +1361,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" ht="12.75" customHeight="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>83</v>
       </c>
@@ -1506,14 +1372,14 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" ht="12.75" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" ht="12.75" customHeight="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="14" t="s">
         <v>86</v>
       </c>
@@ -1524,7 +1390,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" ht="12.75" customHeight="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>77</v>
       </c>
@@ -1535,7 +1401,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" ht="12.75" customHeight="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>80</v>
       </c>
@@ -1546,7 +1412,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" ht="12.75" customHeight="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>83</v>
       </c>
@@ -1557,19 +1423,19 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" ht="12.75" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="12.75" customHeight="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
       <c r="D18" s="14"/>
     </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" ht="12.75" customHeight="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>77</v>
       </c>
@@ -1580,7 +1446,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" ht="12.75" customHeight="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>80</v>
       </c>
@@ -1591,7 +1457,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" ht="12.75" customHeight="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>83</v>
       </c>
@@ -1602,19 +1468,19 @@
         <v>85</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="12.75" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" ht="12.75" customHeight="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="13"/>
       <c r="C25" s="13"/>
       <c r="D25" s="13"/>
     </row>
-    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" ht="12.75" customHeight="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="14" t="s">
         <v>90</v>
       </c>
@@ -1625,7 +1491,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" ht="12.75" customHeight="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>77</v>
       </c>
@@ -1636,7 +1502,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="28" ht="12.75" customHeight="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>80</v>
       </c>
@@ -1647,7 +1513,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="29" ht="12.75" customHeight="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
         <v>83</v>
       </c>
@@ -1658,14 +1524,14 @@
         <v>85</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="30" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" ht="12.75" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="12.75" customHeight="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="13"/>
       <c r="C33" s="13"/>
       <c r="D33" s="13"/>
@@ -1679,7 +1545,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="34" ht="12.75" customHeight="1" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E34" s="2" t="s">
         <v>77</v>
       </c>
@@ -1690,7 +1556,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="35" ht="12.75" customHeight="1" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E35" s="2" t="s">
         <v>80</v>
       </c>
@@ -1701,7 +1567,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="36" ht="12.75" customHeight="1" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E36" s="2" t="s">
         <v>83</v>
       </c>
@@ -1712,14 +1578,14 @@
         <v>85</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="37" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="12.75" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="39" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="12.75" customHeight="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" s="13"/>
       <c r="C40" s="13" t="s">
         <v>93</v>
@@ -1727,7 +1593,7 @@
       <c r="D40" s="13"/>
       <c r="E40" s="13"/>
     </row>
-    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="41" ht="12.75" customHeight="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="13" t="s">
         <v>60</v>
       </c>
@@ -1741,7 +1607,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="42" ht="12.75" customHeight="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
         <v>77</v>
       </c>
@@ -1755,7 +1621,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="43" ht="12.75" customHeight="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
         <v>80</v>
       </c>
@@ -1769,7 +1635,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="44" ht="12.75" customHeight="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
         <v>83</v>
       </c>
@@ -1783,13 +1649,13 @@
         <v>98</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="45" ht="12.75" customHeight="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
     </row>
-    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="46" ht="12.75" customHeight="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
         <v>38</v>
       </c>
@@ -1797,8 +1663,8 @@
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
     </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="47" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" ht="12.75" customHeight="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="14" t="s">
         <v>99</v>
       </c>
@@ -1808,7 +1674,7 @@
       <c r="D48" s="14"/>
       <c r="E48" s="14"/>
     </row>
-    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="49" ht="12.75" customHeight="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49" s="14" t="s">
         <v>94</v>
       </c>
@@ -1820,7 +1686,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="50" ht="12.75" customHeight="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50" s="2" t="s">
         <v>77</v>
       </c>
@@ -1834,7 +1700,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="51" ht="12.75" customHeight="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
         <v>80</v>
       </c>
@@ -1848,7 +1714,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="52" ht="12.75" customHeight="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52" s="2" t="s">
         <v>83</v>
       </c>
@@ -1862,8 +1728,8 @@
         <v>98</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="53" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="12.75" customHeight="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
         <v>47</v>
       </c>
@@ -1871,20 +1737,20 @@
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
     </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="55" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="12.75" customHeight="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B56" s="14"/>
       <c r="C56" s="14"/>
       <c r="D56" s="14"/>
       <c r="E56" s="14"/>
     </row>
-    <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="57" ht="12.75" customHeight="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B57" s="14"/>
       <c r="C57" s="14"/>
       <c r="D57" s="14"/>
       <c r="E57" s="14"/>
     </row>
-    <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="58" ht="12.75" customHeight="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B58" s="2" t="s">
         <v>77</v>
       </c>
@@ -1898,7 +1764,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="59" ht="12.75" customHeight="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B59" s="2" t="s">
         <v>80</v>
       </c>
@@ -1912,7 +1778,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="60" ht="12.75" customHeight="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B60" s="2" t="s">
         <v>83</v>
       </c>
@@ -1926,26 +1792,26 @@
         <v>98</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="12.75" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="63" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="12.75" customHeight="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B64" s="13"/>
       <c r="C64" s="13"/>
       <c r="D64" s="13"/>
       <c r="E64" s="13"/>
     </row>
-    <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="65" ht="12.75" customHeight="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B65" s="13"/>
       <c r="C65" s="13"/>
       <c r="D65" s="13"/>
       <c r="E65" s="13"/>
     </row>
-    <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="66" ht="12.75" customHeight="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66" s="14"/>
       <c r="C66" s="14" t="s">
         <v>69</v>
@@ -1953,7 +1819,7 @@
       <c r="D66" s="14"/>
       <c r="E66" s="14"/>
     </row>
-    <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="67" ht="12.75" customHeight="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B67" s="14" t="s">
         <v>103</v>
       </c>
@@ -1967,7 +1833,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="68" ht="12.75" customHeight="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B68" s="2" t="s">
         <v>77</v>
       </c>
@@ -1981,7 +1847,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="69" ht="12.75" customHeight="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B69" s="2" t="s">
         <v>80</v>
       </c>
@@ -1995,7 +1861,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="70" ht="12.75" customHeight="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B70" s="2" t="s">
         <v>83</v>
       </c>
@@ -2009,14 +1875,14 @@
         <v>98</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="71" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="12.75" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="73" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="12.75" customHeight="1" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B74" s="13"/>
       <c r="C74" s="13"/>
       <c r="D74" s="13"/>
@@ -2028,7 +1894,7 @@
       <c r="H74" s="14"/>
       <c r="I74" s="14"/>
     </row>
-    <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="75" ht="12.75" customHeight="1" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B75" s="13"/>
       <c r="C75" s="13"/>
       <c r="D75" s="13"/>
@@ -2046,7 +1912,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="76" ht="12.75" customHeight="1" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F76" s="2" t="s">
         <v>77</v>
       </c>
@@ -2060,7 +1926,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="77" ht="12.75" customHeight="1" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F77" s="2" t="s">
         <v>80</v>
       </c>
@@ -2074,7 +1940,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="78" ht="12.75" customHeight="1" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F78" s="2" t="s">
         <v>83</v>
       </c>
@@ -2089,10 +1955,9 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
   </headerFooter>
@@ -2100,30 +1965,52 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100" view="normal">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0" defaultColWidth="11.5703125" customHeight="1"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>110</v>
-      </c>
+    <row r="1" ht="12.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="80" zoomScaleNormal="80" view="normal">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0" defaultColWidth="11.53515625" customHeight="1"/>
+  <sheetData>
+    <row r="1" ht="12.75" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;KffffffSeite &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>